<commit_message>
Update BOM GBot Tiny Mark II.xlsx
</commit_message>
<xml_diff>
--- a/BOM GBot Tiny Mark II.xlsx
+++ b/BOM GBot Tiny Mark II.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24536143-6886-4F1E-9E23-0788C015877C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03F37AD-31DA-458E-A5E5-8DD45B038DFE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="76">
   <si>
     <t>Наименование</t>
   </si>
@@ -242,6 +242,12 @@
   </si>
   <si>
     <t>Цена всей сборки</t>
+  </si>
+  <si>
+    <t>Гнездо питания AC-01A</t>
+  </si>
+  <si>
+    <t>https://aliexpress.ru/item/32880955914.html</t>
   </si>
 </sst>
 </file>
@@ -504,6 +510,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -522,30 +546,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -827,10 +833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,618 +850,637 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="21"/>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="8"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="24"/>
       <c r="G2" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="17" t="s">
+      <c r="B5" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="12" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="13">
-        <v>1</v>
-      </c>
-      <c r="C6" s="14">
+      <c r="B6" s="7">
+        <v>1</v>
+      </c>
+      <c r="C6" s="8">
         <v>1829</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="7">
         <f>C6*B6</f>
         <v>1829</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="13"/>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="4">
         <v>728</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="4">
         <f>C7*B7</f>
         <v>2184</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="10">
-        <v>1</v>
-      </c>
-      <c r="C8" s="10">
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4">
         <v>1975</v>
       </c>
-      <c r="D8" s="10">
-        <f t="shared" ref="D8:D26" si="0">C8*B8</f>
+      <c r="D8" s="4">
+        <f t="shared" ref="D8:D27" si="0">C8*B8</f>
         <v>1975</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="10"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="10">
-        <v>1</v>
-      </c>
-      <c r="C9" s="10">
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4">
         <v>742</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="4">
         <f t="shared" si="0"/>
         <v>742</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="10"/>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="10">
-        <v>1</v>
-      </c>
-      <c r="C10" s="10">
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4">
         <v>200</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="4">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="10">
-        <v>1</v>
-      </c>
-      <c r="C11" s="10">
+      <c r="B11" s="4">
+        <v>1</v>
+      </c>
+      <c r="C11" s="4">
         <v>614</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="4">
         <f t="shared" si="0"/>
         <v>614</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="4">
         <v>2</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="4">
         <v>171</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="4">
         <f t="shared" si="0"/>
         <v>342</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="4">
         <v>2</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="4">
         <v>24</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="4">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="10">
-        <v>1</v>
-      </c>
-      <c r="C14" s="10">
+      <c r="B14" s="4">
+        <v>1</v>
+      </c>
+      <c r="C14" s="4">
         <v>24</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="4">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="10">
-        <v>1</v>
-      </c>
-      <c r="C15" s="10">
+      <c r="B15" s="4">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4">
         <v>24</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="4">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="10">
-        <v>1</v>
-      </c>
-      <c r="C16" s="10">
+      <c r="B16" s="4">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4">
         <v>193</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="4">
         <f t="shared" si="0"/>
         <v>193</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="4">
         <v>10</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="4">
         <v>33</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="4">
         <f t="shared" si="0"/>
         <v>330</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="10">
-        <v>1</v>
-      </c>
-      <c r="C18" s="10">
+      <c r="B18" s="4">
+        <v>1</v>
+      </c>
+      <c r="C18" s="4">
         <v>45</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="4">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F18" s="10"/>
+      <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="10">
-        <v>1</v>
-      </c>
-      <c r="C19" s="10">
+      <c r="B19" s="4">
+        <v>1</v>
+      </c>
+      <c r="C19" s="4">
         <v>369</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="4">
         <f t="shared" si="0"/>
         <v>369</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="4" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="10">
-        <v>1</v>
-      </c>
-      <c r="C20" s="10">
+      <c r="B20" s="4">
+        <v>1</v>
+      </c>
+      <c r="C20" s="4">
         <v>1105</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="4">
         <f>C20*B20</f>
         <v>1105</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="4" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="10">
-        <v>1</v>
-      </c>
-      <c r="C21" s="10">
+      <c r="B21" s="4">
+        <v>1</v>
+      </c>
+      <c r="C21" s="4">
         <v>119</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="4">
         <f>C21*B21</f>
         <v>119</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="4" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="10">
-        <v>1</v>
-      </c>
-      <c r="C22" s="10">
+      <c r="B22" s="4">
+        <v>1</v>
+      </c>
+      <c r="C22" s="4">
         <v>16</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="4">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="E22" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F22" s="10"/>
+      <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="10">
-        <v>1</v>
-      </c>
-      <c r="C23" s="10">
+      <c r="B23" s="4">
+        <v>1</v>
+      </c>
+      <c r="C23" s="4">
         <v>767</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="4">
         <f t="shared" si="0"/>
         <v>767</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F23" s="10"/>
+      <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="10">
-        <v>1</v>
-      </c>
-      <c r="C24" s="10">
+      <c r="B24" s="4">
+        <v>1</v>
+      </c>
+      <c r="C24" s="4">
         <v>30</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="4">
         <f>C24*B24</f>
         <v>30</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="4" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="10">
-        <v>1</v>
-      </c>
-      <c r="C25" s="10">
+      <c r="B25" s="4">
+        <v>1</v>
+      </c>
+      <c r="C25" s="4">
         <v>92</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="4">
         <f>C25*B25</f>
         <v>92</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="E25" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="4" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="4">
+        <v>1</v>
+      </c>
+      <c r="C26" s="4">
+        <v>63</v>
+      </c>
+      <c r="D26" s="4">
+        <f>C26*B26</f>
+        <v>63</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="10">
-        <v>1</v>
-      </c>
-      <c r="C26" s="10">
+      <c r="B27" s="4">
+        <v>1</v>
+      </c>
+      <c r="C27" s="4">
         <v>500</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D27" s="4">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="10">
-        <v>1</v>
-      </c>
-      <c r="C27" s="10">
+      <c r="B28" s="4">
+        <v>1</v>
+      </c>
+      <c r="C28" s="4">
         <v>5000</v>
       </c>
-      <c r="D27" s="10">
-        <f>C27*B27</f>
+      <c r="D28" s="4">
+        <f>C28*B28</f>
         <v>5000</v>
       </c>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-    </row>
-    <row r="30" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B30" s="9"/>
-      <c r="C30" s="25" t="s">
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+    </row>
+    <row r="31" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B31" s="3"/>
+      <c r="C31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="26">
-        <f>SUM(D6:D27)</f>
-        <v>16548</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="D31" s="18">
+        <f>SUM(D6:D28)</f>
+        <v>16611</v>
+      </c>
+      <c r="E31" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="19" t="s">
+    <row r="33" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B33" s="10">
-        <v>1</v>
-      </c>
-      <c r="C33" s="10">
+      <c r="B34" s="4">
+        <v>1</v>
+      </c>
+      <c r="C34" s="4">
         <v>2323</v>
       </c>
-      <c r="D33" s="10">
-        <f>B33*C33</f>
+      <c r="D34" s="4">
+        <f>B34*C34</f>
         <v>2323</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E34" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F33" s="10" t="s">
+      <c r="F34" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="11" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="10">
-        <v>1</v>
-      </c>
-      <c r="C35" s="10">
+      <c r="B36" s="4">
+        <v>1</v>
+      </c>
+      <c r="C36" s="4">
         <v>4992</v>
       </c>
-      <c r="D35" s="10">
-        <f>B35*C35</f>
+      <c r="D36" s="4">
+        <f>B36*C36</f>
         <v>4992</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E36" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F35" s="10" t="s">
+      <c r="F36" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B36" s="10">
-        <v>1</v>
-      </c>
-      <c r="C36" s="10">
+      <c r="B37" s="4">
+        <v>1</v>
+      </c>
+      <c r="C37" s="4">
         <v>773</v>
       </c>
-      <c r="D36" s="10">
-        <f>B36*C36</f>
+      <c r="D37" s="4">
+        <f>B37*C37</f>
         <v>773</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E37" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F36" s="10"/>
-    </row>
-    <row r="38" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C38" s="25" t="s">
+      <c r="F37" s="4"/>
+    </row>
+    <row r="39" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C39" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="26">
-        <f>SUM(D35:D36)</f>
+      <c r="D39" s="18">
+        <f>SUM(D36:D37)</f>
         <v>5765</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+    <row r="41" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="22" t="s">
+      <c r="B41" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="C40" s="23"/>
-      <c r="D40" s="24">
-        <f>D30+D38</f>
-        <v>22313</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="16">
+        <f>D31+D39</f>
+        <v>22376</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:F2"/>
-    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E6" r:id="rId1" xr:uid="{30FF7445-DA6B-426E-94A7-7F83247EFB61}"/>

</xml_diff>